<commit_message>
Unit Test Energy Impact
</commit_message>
<xml_diff>
--- a/viz_scripts/auxiliary_files/cost_time.xlsx
+++ b/viz_scripts/auxiliary_files/cost_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syoung3/GitHub/em-public-dashboard/viz_scripts/auxiliary_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD3DF60B-67AA-434E-B8A9-746E21D1CBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0FD0FCBE-F52E-BE41-B6D3-611495103B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
   </bookViews>
@@ -931,7 +931,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -994,7 +994,8 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <f>3.298*1/25.5</f>
+        <v>0.12933333333333333</v>
       </c>
       <c r="C4">
         <v>0</v>

</xml_diff>